<commit_message>
mixed effects models of treatment effects added
</commit_message>
<xml_diff>
--- a/data/alkalinity/fl_ybc_oct_alkalinity.xlsx
+++ b/data/alkalinity/fl_ybc_oct_alkalinity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alice.carter\Dropbox\Kirby_priming\DOC_priming\data\alkalinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A238B3B-4681-447B-A109-744CD3CE0D07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD7B4CF-25F2-402D-B64D-048AF03BDCD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" xr2:uid="{424C5B6D-93D5-4887-9A10-0CC269547B3F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="20">
   <si>
     <t>samplenum</t>
   </si>
@@ -54,9 +54,6 @@
     <t>LW</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>vol h20</t>
   </si>
   <si>
@@ -67,6 +64,27 @@
   </si>
   <si>
     <t>probe still questionable</t>
+  </si>
+  <si>
+    <t>starting_pH</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>CNP</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>overshot</t>
   </si>
 </sst>
 </file>
@@ -419,20 +437,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD602AE-1D90-447C-A930-661371337FD7}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,22 +468,25 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -475,20 +497,20 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="I2">
-        <f>(20*F2)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <f t="shared" ref="K2:K20" si="0">(20*G2)/50</f>
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -499,192 +521,1028 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
         <v>4.1900000000000004</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>4.57</v>
       </c>
-      <c r="I3">
-        <f>(20*F3)/50</f>
+      <c r="K3">
+        <f>(20*G3)/F3</f>
         <v>1.6760000000000002</v>
       </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>4.16</v>
+      </c>
+      <c r="H4">
+        <v>7.96</v>
+      </c>
       <c r="I4">
-        <f>(20*F4)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.49</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K33" si="1">(20*G4)/F4</f>
+        <v>1.6640000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>4.16</v>
+      </c>
+      <c r="H5">
+        <v>7.78</v>
+      </c>
       <c r="I5">
-        <f>(20*F5)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>1.6640000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="H6">
+        <v>8.0500000000000007</v>
+      </c>
       <c r="I6">
-        <f>(20*F6)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>1.6760000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>4.12</v>
+      </c>
+      <c r="H7">
+        <v>7.91</v>
+      </c>
       <c r="I7">
-        <f>(20*F7)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.49</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>1.6480000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H8">
+        <v>7.78</v>
+      </c>
       <c r="I8">
-        <f>(20*F8)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.3</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>1.7079999999999997</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>4.16</v>
+      </c>
+      <c r="H9">
+        <v>7.81</v>
+      </c>
       <c r="I9">
-        <f>(20*F9)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.45</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>1.6640000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>3.86</v>
+      </c>
+      <c r="H10">
+        <v>7.68</v>
+      </c>
       <c r="I10">
-        <f>(20*F10)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.47</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>1.544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>3.77</v>
+      </c>
+      <c r="H11">
+        <v>7.78</v>
+      </c>
       <c r="I11">
-        <f>(20*F11)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.47</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>1.508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>3.82</v>
+      </c>
+      <c r="H12">
+        <v>7.87</v>
+      </c>
       <c r="I12">
-        <f>(20*F12)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>1.5279999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>3.8</v>
+      </c>
+      <c r="H13">
+        <v>7.8</v>
+      </c>
       <c r="I13">
-        <f>(20*F13)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>3.83</v>
+      </c>
+      <c r="H14">
+        <v>7.79</v>
+      </c>
       <c r="I14">
-        <f>(20*F14)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="K14">
+        <f>(20*G15)/F14</f>
+        <v>1.4960000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>3.74</v>
+      </c>
+      <c r="H15">
+        <v>7.82</v>
+      </c>
       <c r="I15">
-        <f>(20*F15)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.49</v>
+      </c>
+      <c r="K15">
+        <f>(20*G16)/F15</f>
+        <v>1.5119999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>3.78</v>
+      </c>
+      <c r="H16">
+        <v>7.7</v>
+      </c>
       <c r="I16">
-        <f>(20*F16)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.45</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:K17" si="2">(20*G17)/F16</f>
+        <v>1.5039999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>3.76</v>
+      </c>
+      <c r="H17">
+        <v>7.78</v>
+      </c>
       <c r="I17">
-        <f>(20*F17)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.47</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H18">
+        <v>7.99</v>
+      </c>
       <c r="I18">
-        <f>(20*F18)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="H19">
+        <v>7.93</v>
+      </c>
       <c r="I19">
-        <f>(20*F19)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.34</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>1.6760000000000002</v>
+      </c>
+      <c r="L19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>4.18</v>
+      </c>
+      <c r="H20">
+        <v>7.94</v>
+      </c>
       <c r="I20">
-        <f>(20*F20)/50</f>
-        <v>0</v>
+        <v>4.51</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H21">
+        <v>7.84</v>
+      </c>
+      <c r="I21">
+        <v>4.49</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="H22">
+        <v>7.99</v>
+      </c>
+      <c r="I22">
+        <v>4.5</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>1.6559999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="H23">
+        <v>7.84</v>
+      </c>
+      <c r="I23">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>1.6559999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>4.2</v>
+      </c>
+      <c r="H24">
+        <v>7.84</v>
+      </c>
+      <c r="I24">
+        <v>4.5</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H25">
+        <v>7.79</v>
+      </c>
+      <c r="I25">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>3.7</v>
+      </c>
+      <c r="H26">
+        <v>7.85</v>
+      </c>
+      <c r="I26">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>3.71</v>
+      </c>
+      <c r="H27">
+        <v>7.8</v>
+      </c>
+      <c r="I27">
+        <v>4.51</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>1.484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>45</v>
+      </c>
+      <c r="G28">
+        <v>3.57</v>
+      </c>
+      <c r="H28">
+        <v>7.85</v>
+      </c>
+      <c r="I28">
+        <v>4.05</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>1.5866666666666664</v>
+      </c>
+      <c r="L28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>3.7</v>
+      </c>
+      <c r="H29">
+        <v>7.8</v>
+      </c>
+      <c r="I29">
+        <v>4.53</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>3.74</v>
+      </c>
+      <c r="H30">
+        <v>7.86</v>
+      </c>
+      <c r="I30">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>1.4960000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>3.7</v>
+      </c>
+      <c r="H31">
+        <v>7.79</v>
+      </c>
+      <c r="I31">
+        <v>4.5</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
+        <v>4.01</v>
+      </c>
+      <c r="H32">
+        <v>7.84</v>
+      </c>
+      <c r="I32">
+        <v>4.07</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>1.6039999999999999</v>
+      </c>
+      <c r="L32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45203</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33">
+        <v>3.68</v>
+      </c>
+      <c r="H33">
+        <v>7.73</v>
+      </c>
+      <c r="I33">
+        <v>4.46</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>1.4720000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>